<commit_message>
feat: add de lang
</commit_message>
<xml_diff>
--- a/Automotive digital showroom_localization-ger-DE.xlsx
+++ b/Automotive digital showroom_localization-ger-DE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://getac-my.sharepoint.com/personal/eric_yeh_getac_com/Documents/EU-Getac/Marketing Europe/Events and exHibitions/Digital Trade Show/AUTOMOTIVE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bonnie\Project\2021\2__Automotive\LP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{6FF6FAD0-2696-491E-85DA-C20D9D78870C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37019001-D969-4424-89EA-2BC798B81724}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{79022609-F502-2843-86B9-FF0EE491FBD4}"/>
+    <workbookView xWindow="20376" yWindow="-120" windowWidth="29040" windowHeight="15996"/>
   </bookViews>
   <sheets>
     <sheet name="Inhalt 3D-Bereich" sheetId="3" r:id="rId1"/>
@@ -2449,18 +2448,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2674,7 +2673,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2985,323 +2984,324 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4410C8DC-4799-4C08-98A5-2E627E6B0177}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="53" customWidth="1"/>
-    <col min="3" max="3" width="67.375" customWidth="1"/>
-    <col min="4" max="4" width="71.5" customWidth="1"/>
-    <col min="5" max="5" width="74.5" customWidth="1"/>
-    <col min="6" max="6" width="61.5" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="14"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="5" max="5" width="67.33203125" customWidth="1"/>
+    <col min="6" max="6" width="71.44140625" customWidth="1"/>
+    <col min="7" max="7" width="74.44140625" customWidth="1"/>
+    <col min="8" max="8" width="61.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="3:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="C1" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="3:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="24"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="362.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="3:8" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="267.75">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="3:8" ht="265.2" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="252">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="3:8" ht="265.2" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="173.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="3:8" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="220.5">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="3:8" ht="234" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="189">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="3:8" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="236.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="3:8" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="204.75">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="3:8" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="267.75">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="3:8" ht="265.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="236.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="3:8" ht="234" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="252">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="3:8" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="236.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="3:8" ht="234" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="283.5">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="3:8" ht="280.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="H15" s="8" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3310,20 +3310,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F3552A-438E-4F65-9D8C-BF1513719D8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.25" customWidth="1"/>
-    <col min="2" max="2" width="64.875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="57.21875" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="14" customFormat="1">
+    <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>147</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>104</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="47.25">
+    <row r="3" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>105</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>106</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>107</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="78.75">
+    <row r="6" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>108</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>109</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="78.75">
+    <row r="8" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>110</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>111</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="94.5">
+    <row r="10" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>112</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>113</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="78.75">
+    <row r="12" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>114</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>115</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="94.5">
+    <row r="14" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>116</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>117</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="78.75">
+    <row r="16" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>118</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>119</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="94.5">
+    <row r="18" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>120</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>121</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="94.5">
+    <row r="20" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>122</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="31.5">
+    <row r="21" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>123</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="47.25">
+    <row r="22" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>124</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>125</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>126</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>127</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>128</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>129</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="110.25">
+    <row r="28" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>130</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>131</v>
       </c>
@@ -3555,11 +3555,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="18"/>
     </row>
-    <row r="31" spans="1:2" ht="63">
+    <row r="31" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>132</v>
       </c>
@@ -3567,11 +3567,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="18"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>133</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="31.5">
+    <row r="34" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>134</v>
       </c>
@@ -3587,11 +3587,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="18"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>135</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="47.25">
+    <row r="37" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>136</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>137</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>138</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>139</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>140</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
         <v>141</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>142</v>
       </c>
@@ -3655,15 +3655,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="22"/>
       <c r="B44" s="18"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="22"/>
       <c r="B45" s="18"/>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
         <v>143</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>144</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
         <v>145</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>146</v>
       </c>
@@ -3709,15 +3709,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009692DBEC0A2E4F428E3CB37AF93C8C0A" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a4d1e959dc07e3a4d68d206d29a82cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="992915c6-1938-47c0-9c76-71ba88e3d674" xmlns:ns3="474cc9fd-7d94-4ddb-9132-d1ce0f0fdcce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d34ce3df8c33ed6b6d86e04e4b13c4f" ns2:_="" ns3:_="">
     <xsd:import namespace="992915c6-1938-47c0-9c76-71ba88e3d674"/>
@@ -3928,6 +3919,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE50E54-1820-494A-A8E7-11724CA6F303}">
   <ds:schemaRefs>
@@ -3946,14 +3946,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98676BB0-AF15-455A-9D9E-8BC46C5236DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6267EF65-F57C-4C89-88F6-4A0B6C2B628E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3970,4 +3962,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98676BB0-AF15-455A-9D9E-8BC46C5236DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>